<commit_message>
- 품목 헤드, cpp 나눔 - handler .h .cpp 생성 - 메인문 나눔
</commit_message>
<xml_diff>
--- a/MiniProject/자료들/메뉴구성 및 결과.xlsx
+++ b/MiniProject/자료들/메뉴구성 및 결과.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PKNU\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_IoT\Cpp_MiniProject\Cpp_Miniproject\MiniProject\자료들\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;공정번호선택&gt; -&gt; 해당공정에서 발생한 불량정보 출력</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>결과 및 프로세스</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -217,10 +213,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>4) 뒤로가기</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1) 생산계획등록</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,6 +222,14 @@
   </si>
   <si>
     <t>3) 뒤로가기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;오류가 발생한 제품의 정보 및 오류정보 출력&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">4) 뒤로가기    </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,21 +683,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -714,15 +699,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -779,6 +755,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -788,10 +770,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1078,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1087,7 @@
     <col min="2" max="2" width="28.75" customWidth="1"/>
     <col min="3" max="3" width="50.625" customWidth="1"/>
     <col min="4" max="4" width="47.125" customWidth="1"/>
-    <col min="5" max="5" width="29.25" customWidth="1"/>
+    <col min="5" max="5" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -1099,227 +1099,227 @@
         <v>5</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="35"/>
-      <c r="E3" s="31"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="23"/>
     </row>
     <row r="4" spans="2:5" ht="33" x14ac:dyDescent="0.3">
-      <c r="B4" s="10"/>
+      <c r="B4" s="40"/>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="40" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="32" t="s">
+      <c r="D4" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="32"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="12"/>
-      <c r="C6" s="36" t="s">
+      <c r="B6" s="41"/>
+      <c r="C6" s="28" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="30"/>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="40"/>
+      <c r="C8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="37"/>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="20" t="s">
+      <c r="D8" s="6"/>
+      <c r="E8" s="24"/>
+    </row>
+    <row r="9" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="43"/>
+      <c r="C9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="38"/>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B8" s="10"/>
-      <c r="C8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="32"/>
-    </row>
-    <row r="9" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
-      <c r="C9" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="33"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" spans="2:5" ht="116.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="39"/>
+      <c r="C11" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="31"/>
     </row>
     <row r="12" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="13" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="44" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="45"/>
+      <c r="D13" s="46"/>
+    </row>
+    <row r="14" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="23"/>
-    </row>
-    <row r="14" spans="2:5" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="25" t="s">
+      <c r="C16" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B15" s="28" t="s">
+      <c r="D16" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B17" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B18" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="C20" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.3">
-      <c r="B16" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D16" s="32" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B17" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="32" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B18" s="29" t="s">
+    <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B19" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B20" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="32" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>21</v>
+      <c r="C21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="24" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
+      <c r="B24" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="37"/>
+      <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="D25" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="B26" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="C26" s="11" t="s">
         <v>42</v>
+      </c>
+      <c r="D26" s="35" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>